<commit_message>
Update metadata for calibration protocol
</commit_message>
<xml_diff>
--- a/examples/protocols/multicolor-particle-calibration/metadata/measure_fluourescence1.xlsx
+++ b/examples/protocols/multicolor-particle-calibration/metadata/measure_fluourescence1.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danbryce/Documents/sift/xplan/external/labop/examples/protocols/multicolor-particle-calibration/metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bbartley/Dev/git/sd2/paml/examples/protocols/multicolor-particle-calibration/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C8FDA20-AB7D-3046-A140-E45C146E14A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D86EAA0-4801-5449-8503-A1097F755B2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="106520" yWindow="7800" windowWidth="29640" windowHeight="20260" xr2:uid="{E2C2EB55-5F9A-0D47-B3AE-0000058D112A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20340" xr2:uid="{E2C2EB55-5F9A-0D47-B3AE-0000058D112A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="115">
   <si>
     <t>A1</t>
   </si>
@@ -147,22 +147,238 @@
     <t>sample</t>
   </si>
   <si>
-    <t>fluorescene</t>
-  </si>
-  <si>
-    <t>nanocym</t>
-  </si>
-  <si>
-    <t>water</t>
-  </si>
-  <si>
-    <t>pbs</t>
-  </si>
-  <si>
-    <t>sulforhodamine101</t>
-  </si>
-  <si>
-    <t>cascadeBlue</t>
+    <t>fluoroscein (uM)</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>D6</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>D9</t>
+  </si>
+  <si>
+    <t>D10</t>
+  </si>
+  <si>
+    <t>D11</t>
+  </si>
+  <si>
+    <t>D12</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>E2</t>
+  </si>
+  <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>E5</t>
+  </si>
+  <si>
+    <t>E6</t>
+  </si>
+  <si>
+    <t>E7</t>
+  </si>
+  <si>
+    <t>E8</t>
+  </si>
+  <si>
+    <t>E9</t>
+  </si>
+  <si>
+    <t>E10</t>
+  </si>
+  <si>
+    <t>E11</t>
+  </si>
+  <si>
+    <t>E12</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>F5</t>
+  </si>
+  <si>
+    <t>F6</t>
+  </si>
+  <si>
+    <t>F7</t>
+  </si>
+  <si>
+    <t>F8</t>
+  </si>
+  <si>
+    <t>F9</t>
+  </si>
+  <si>
+    <t>F10</t>
+  </si>
+  <si>
+    <t>F11</t>
+  </si>
+  <si>
+    <t>F12</t>
+  </si>
+  <si>
+    <t>G1</t>
+  </si>
+  <si>
+    <t>G2</t>
+  </si>
+  <si>
+    <t>G3</t>
+  </si>
+  <si>
+    <t>G4</t>
+  </si>
+  <si>
+    <t>G5</t>
+  </si>
+  <si>
+    <t>G6</t>
+  </si>
+  <si>
+    <t>G7</t>
+  </si>
+  <si>
+    <t>G8</t>
+  </si>
+  <si>
+    <t>G9</t>
+  </si>
+  <si>
+    <t>G10</t>
+  </si>
+  <si>
+    <t>G11</t>
+  </si>
+  <si>
+    <t>G12</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>H3</t>
+  </si>
+  <si>
+    <t>H4</t>
+  </si>
+  <si>
+    <t>H5</t>
+  </si>
+  <si>
+    <t>H6</t>
+  </si>
+  <si>
+    <t>H7</t>
+  </si>
+  <si>
+    <t>H8</t>
+  </si>
+  <si>
+    <t>H9</t>
+  </si>
+  <si>
+    <t>H10</t>
+  </si>
+  <si>
+    <t>H11</t>
+  </si>
+  <si>
+    <t>H12</t>
+  </si>
+  <si>
+    <t>sulforhodamine (uM)</t>
+  </si>
+  <si>
+    <t>cascade blue (uM)</t>
+  </si>
+  <si>
+    <t>NanoCym beads (1/mL)</t>
+  </si>
+  <si>
+    <t>double distilled water (uL)</t>
+  </si>
+  <si>
+    <t>PBS (uL)</t>
   </si>
 </sst>
 </file>
@@ -274,7 +490,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -589,158 +805,2328 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F49C91B-78E4-C744-87BD-E5730306C71E}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="111" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="7" width="10.83203125" style="7"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>40</v>
+      <c r="C1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="B3">
+        <f>B2/2</f>
+        <v>2.5</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>200</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="B4">
+        <f>B3/2</f>
+        <v>1.25</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>200</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
+      <c r="B5">
+        <f t="shared" ref="B5:B13" si="0">B4/2</f>
+        <v>0.625</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>200</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>0.3125</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>200</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>0.15625</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>200</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>7.8125E-2</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>200</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>3.90625E-2</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>200</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>1.953125E-2</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>200</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>9.765625E-3</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>200</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>4.8828125E-3</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>200</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>200</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>200</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
+      <c r="B15">
+        <f>B14/2</f>
+        <v>2.5</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>200</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <f>B15/2</f>
+        <v>1.25</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <f t="shared" ref="B17:B24" si="1">B16/2</f>
+        <v>0.625</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <f t="shared" si="1"/>
+        <v>0.3125</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <f t="shared" si="1"/>
+        <v>0.15625</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <f t="shared" si="1"/>
+        <v>7.8125E-2</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <f t="shared" si="1"/>
+        <v>3.90625E-2</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <f t="shared" si="1"/>
+        <v>1.953125E-2</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <f t="shared" si="1"/>
+        <v>9.765625E-3</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B24">
+        <f t="shared" si="1"/>
+        <v>4.8828125E-3</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <f>C26/2</f>
+        <v>0.5</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <f t="shared" ref="C28:C37" si="2">C27/2</f>
+        <v>0.25</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="2"/>
+        <v>0.125</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="2"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="2"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="2"/>
+        <v>1.5625E-2</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="2"/>
+        <v>7.8125E-3</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="2"/>
+        <v>3.90625E-3</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="2"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>48</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="2"/>
+        <v>9.765625E-4</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>50</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>51</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <f>C38/2</f>
+        <v>0.5</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>52</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <f t="shared" ref="C40:C48" si="3">C39/2</f>
+        <v>0.25</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>53</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="3"/>
+        <v>0.125</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>54</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="3"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="3"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>56</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="3"/>
+        <v>1.5625E-2</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>57</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="3"/>
+        <v>7.8125E-3</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>58</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="3"/>
+        <v>3.90625E-3</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>59</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="3"/>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>60</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="3"/>
+        <v>9.765625E-4</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>61</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>62</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>5</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>200</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>63</v>
+      </c>
+      <c r="B51">
+        <v>0</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <f>D50/2</f>
+        <v>2.5</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <v>200</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>64</v>
+      </c>
+      <c r="B52">
+        <v>0</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <f>D51/2</f>
+        <v>1.25</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52">
+        <v>200</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>65</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <f t="shared" ref="D53:D60" si="4">D52/2</f>
+        <v>0.625</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>200</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>66</v>
+      </c>
+      <c r="B54">
+        <v>0</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="4"/>
+        <v>0.3125</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>200</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>67</v>
+      </c>
+      <c r="B55">
+        <v>0</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="4"/>
+        <v>0.15625</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>200</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>68</v>
+      </c>
+      <c r="B56">
+        <v>0</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="4"/>
+        <v>7.8125E-2</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>200</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>69</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="4"/>
+        <v>3.90625E-2</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>200</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>70</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="4"/>
+        <v>1.953125E-2</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>200</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>71</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="4"/>
+        <v>9.765625E-3</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <v>200</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>72</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="4"/>
+        <v>4.8828125E-3</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>200</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>73</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>200</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>74</v>
+      </c>
+      <c r="B62">
+        <v>0</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>5</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>200</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>75</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <f>D62/2</f>
+        <v>2.5</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>200</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>76</v>
+      </c>
+      <c r="B64">
+        <v>0</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <f t="shared" ref="D64:D72" si="5">D63/2</f>
+        <v>1.25</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>200</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>77</v>
+      </c>
+      <c r="B65">
+        <v>0</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="5"/>
+        <v>0.625</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>200</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>78</v>
+      </c>
+      <c r="B66">
+        <v>0</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="5"/>
+        <v>0.3125</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66">
+        <v>200</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>79</v>
+      </c>
+      <c r="B67">
+        <v>0</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <f t="shared" si="5"/>
+        <v>0.15625</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <v>200</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>80</v>
+      </c>
+      <c r="B68">
+        <v>0</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="5"/>
+        <v>7.8125E-2</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68">
+        <v>200</v>
+      </c>
+      <c r="G68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>81</v>
+      </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="5"/>
+        <v>3.90625E-2</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>200</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>82</v>
+      </c>
+      <c r="B70">
+        <v>0</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="5"/>
+        <v>1.953125E-2</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <v>200</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>83</v>
+      </c>
+      <c r="B71">
+        <v>0</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="5"/>
+        <v>9.765625E-3</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <v>200</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>84</v>
+      </c>
+      <c r="B72">
+        <v>0</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <f t="shared" si="5"/>
+        <v>4.8828125E-3</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <v>200</v>
+      </c>
+      <c r="G72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>85</v>
+      </c>
+      <c r="B73">
+        <v>0</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73">
+        <v>200</v>
+      </c>
+      <c r="G73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>86</v>
+      </c>
+      <c r="B74">
+        <v>0</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74" s="7">
+        <v>1500000000</v>
+      </c>
+      <c r="F74">
+        <v>200</v>
+      </c>
+      <c r="G74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>87</v>
+      </c>
+      <c r="B75">
+        <v>0</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+      <c r="E75" s="7">
+        <f>E74/2</f>
+        <v>750000000</v>
+      </c>
+      <c r="F75">
+        <v>200</v>
+      </c>
+      <c r="G75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>88</v>
+      </c>
+      <c r="B76">
+        <v>0</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+      <c r="E76" s="7">
+        <f t="shared" ref="E76:E84" si="6">E75/2</f>
+        <v>375000000</v>
+      </c>
+      <c r="F76">
+        <v>200</v>
+      </c>
+      <c r="G76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>89</v>
+      </c>
+      <c r="B77">
+        <v>0</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+      <c r="E77" s="7">
+        <f t="shared" si="6"/>
+        <v>187500000</v>
+      </c>
+      <c r="F77">
+        <v>200</v>
+      </c>
+      <c r="G77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>90</v>
+      </c>
+      <c r="B78">
+        <v>0</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
+      <c r="E78" s="7">
+        <f t="shared" si="6"/>
+        <v>93750000</v>
+      </c>
+      <c r="F78">
+        <v>200</v>
+      </c>
+      <c r="G78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>91</v>
+      </c>
+      <c r="B79">
+        <v>0</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
+      <c r="D79">
+        <v>0</v>
+      </c>
+      <c r="E79" s="7">
+        <f t="shared" si="6"/>
+        <v>46875000</v>
+      </c>
+      <c r="F79">
+        <v>200</v>
+      </c>
+      <c r="G79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>92</v>
+      </c>
+      <c r="B80">
+        <v>0</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+      <c r="E80" s="7">
+        <f t="shared" si="6"/>
+        <v>23437500</v>
+      </c>
+      <c r="F80">
+        <v>200</v>
+      </c>
+      <c r="G80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>93</v>
+      </c>
+      <c r="B81">
+        <v>0</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="D81">
+        <v>0</v>
+      </c>
+      <c r="E81" s="7">
+        <f t="shared" si="6"/>
+        <v>11718750</v>
+      </c>
+      <c r="F81">
+        <v>200</v>
+      </c>
+      <c r="G81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>94</v>
+      </c>
+      <c r="B82">
+        <v>0</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
+      </c>
+      <c r="D82">
+        <v>0</v>
+      </c>
+      <c r="E82" s="7">
+        <f t="shared" si="6"/>
+        <v>5859375</v>
+      </c>
+      <c r="F82">
+        <v>200</v>
+      </c>
+      <c r="G82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>95</v>
+      </c>
+      <c r="B83">
+        <v>0</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="E83" s="7">
+        <f t="shared" si="6"/>
+        <v>2929687.5</v>
+      </c>
+      <c r="F83">
+        <v>200</v>
+      </c>
+      <c r="G83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>96</v>
+      </c>
+      <c r="B84">
+        <v>0</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+      <c r="D84">
+        <v>0</v>
+      </c>
+      <c r="E84" s="7">
+        <f t="shared" si="6"/>
+        <v>1464843.75</v>
+      </c>
+      <c r="F84">
+        <v>200</v>
+      </c>
+      <c r="G84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>97</v>
+      </c>
+      <c r="B85">
+        <v>0</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+      <c r="F85">
+        <v>200</v>
+      </c>
+      <c r="G85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>98</v>
+      </c>
+      <c r="B86">
+        <v>0</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
+      </c>
+      <c r="D86">
+        <v>0</v>
+      </c>
+      <c r="E86" s="7">
+        <v>1500000000</v>
+      </c>
+      <c r="F86">
+        <v>200</v>
+      </c>
+      <c r="G86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>99</v>
+      </c>
+      <c r="B87">
+        <v>0</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="D87">
+        <v>0</v>
+      </c>
+      <c r="E87" s="7">
+        <f>E86/2</f>
+        <v>750000000</v>
+      </c>
+      <c r="F87">
+        <v>200</v>
+      </c>
+      <c r="G87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>100</v>
+      </c>
+      <c r="B88">
+        <v>0</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+      <c r="E88" s="7">
+        <f t="shared" ref="E88:E97" si="7">E87/2</f>
+        <v>375000000</v>
+      </c>
+      <c r="F88">
+        <v>200</v>
+      </c>
+      <c r="G88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>101</v>
+      </c>
+      <c r="B89">
+        <v>0</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+      <c r="D89">
+        <v>0</v>
+      </c>
+      <c r="E89" s="7">
+        <f t="shared" si="7"/>
+        <v>187500000</v>
+      </c>
+      <c r="F89">
+        <v>200</v>
+      </c>
+      <c r="G89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>102</v>
+      </c>
+      <c r="B90">
+        <v>0</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
+      </c>
+      <c r="D90">
+        <v>0</v>
+      </c>
+      <c r="E90" s="7">
+        <f t="shared" si="7"/>
+        <v>93750000</v>
+      </c>
+      <c r="F90">
+        <v>200</v>
+      </c>
+      <c r="G90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>103</v>
+      </c>
+      <c r="B91">
+        <v>0</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
+      </c>
+      <c r="D91">
+        <v>0</v>
+      </c>
+      <c r="E91" s="7">
+        <f t="shared" si="7"/>
+        <v>46875000</v>
+      </c>
+      <c r="F91">
+        <v>200</v>
+      </c>
+      <c r="G91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>104</v>
+      </c>
+      <c r="B92">
+        <v>0</v>
+      </c>
+      <c r="C92">
+        <v>0</v>
+      </c>
+      <c r="D92">
+        <v>0</v>
+      </c>
+      <c r="E92" s="7">
+        <f t="shared" si="7"/>
+        <v>23437500</v>
+      </c>
+      <c r="F92">
+        <v>200</v>
+      </c>
+      <c r="G92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>105</v>
+      </c>
+      <c r="B93">
+        <v>0</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+      <c r="E93" s="7">
+        <f t="shared" si="7"/>
+        <v>11718750</v>
+      </c>
+      <c r="F93">
+        <v>200</v>
+      </c>
+      <c r="G93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>106</v>
+      </c>
+      <c r="B94">
+        <v>0</v>
+      </c>
+      <c r="C94">
+        <v>0</v>
+      </c>
+      <c r="D94">
+        <v>0</v>
+      </c>
+      <c r="E94" s="7">
+        <f t="shared" si="7"/>
+        <v>5859375</v>
+      </c>
+      <c r="F94">
+        <v>200</v>
+      </c>
+      <c r="G94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>107</v>
+      </c>
+      <c r="B95">
+        <v>0</v>
+      </c>
+      <c r="C95">
+        <v>0</v>
+      </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
+      <c r="E95" s="7">
+        <f t="shared" si="7"/>
+        <v>2929687.5</v>
+      </c>
+      <c r="F95">
+        <v>200</v>
+      </c>
+      <c r="G95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>108</v>
+      </c>
+      <c r="B96">
+        <v>0</v>
+      </c>
+      <c r="C96">
+        <v>0</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+      <c r="E96" s="7">
+        <f t="shared" si="7"/>
+        <v>1464843.75</v>
+      </c>
+      <c r="F96">
+        <v>200</v>
+      </c>
+      <c r="G96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>109</v>
+      </c>
+      <c r="B97">
+        <v>0</v>
+      </c>
+      <c r="C97">
+        <v>0</v>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+      <c r="E97" s="7">
+        <f t="shared" si="7"/>
+        <v>732421.875</v>
+      </c>
+      <c r="F97">
+        <v>200</v>
+      </c>
+      <c r="G97">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>